<commit_message>
upload all lab solution
</commit_message>
<xml_diff>
--- a/lab planner CSJS 2025.xlsx
+++ b/lab planner CSJS 2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BCA - 4\Client Side Scripting using JavaScript\imp docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mr.aniruddh/Desktop/ME/TA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D785582E-4F05-44EC-8FAC-2C3734CDD6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383B29B1-0D89-F04F-81DA-154EA6264C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="580" windowWidth="25600" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -856,19 +856,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="93.88671875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>36</v>
       </c>
@@ -882,7 +882,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -896,7 +896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -910,7 +910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -924,7 +924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="144" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -938,7 +938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -952,7 +952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="115.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="115.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -966,7 +966,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -980,7 +980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -994,7 +994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="85.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="59.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="88.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="85.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="46.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>22</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="56.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>27</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>28</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>29</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>30</v>
       </c>
@@ -1316,14 +1316,14 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" ht="128" x14ac:dyDescent="0.2">
       <c r="B2" s="9" t="s">
         <v>55</v>
       </c>

</xml_diff>